<commit_message>
CLASSIFICATION column name changed to INFORMATIONDOMAIN in Excel files
</commit_message>
<xml_diff>
--- a/test_files/Code_filter.xlsx
+++ b/test_files/Code_filter.xlsx
@@ -74,37 +74,37 @@
     <t>T53</t>
   </si>
   <si>
+    <t>Testi03</t>
+  </si>
+  <si>
+    <t>T54</t>
+  </si>
+  <si>
+    <t>Testi04</t>
+  </si>
+  <si>
+    <t>T55</t>
+  </si>
+  <si>
+    <t>Testi05</t>
+  </si>
+  <si>
+    <t>T56</t>
+  </si>
+  <si>
+    <t>Testi06</t>
+  </si>
+  <si>
+    <t>T57</t>
+  </si>
+  <si>
+    <t>Testi07</t>
+  </si>
+  <si>
     <t>ORGANIZATION</t>
   </si>
   <si>
-    <t>Testi03</t>
-  </si>
-  <si>
-    <t>T54</t>
-  </si>
-  <si>
-    <t>Testi04</t>
-  </si>
-  <si>
-    <t>T55</t>
-  </si>
-  <si>
-    <t>Testi05</t>
-  </si>
-  <si>
-    <t>T56</t>
-  </si>
-  <si>
-    <t>Testi06</t>
-  </si>
-  <si>
-    <t>T57</t>
-  </si>
-  <si>
-    <t>Testi07</t>
-  </si>
-  <si>
-    <t>CLASSIFICATION</t>
+    <t>INFORMATIONDOMAIN</t>
   </si>
   <si>
     <t>VERSION</t>
@@ -197,10 +197,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -248,81 +248,81 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -339,15 +339,15 @@
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="1"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
       <c r="P2" s="6"/>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="2"/>
       <c r="R2" s="7"/>
       <c r="S2" s="7"/>
       <c r="T2" s="6"/>
@@ -1444,64 +1444,64 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1"/>

</xml_diff>